<commit_message>
Update weekly facility assessment export with daily info
</commit_message>
<xml_diff>
--- a/inst/extdata/wfa_dict.xlsx
+++ b/inst/extdata/wfa_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>old</t>
   </si>
@@ -101,7 +101,61 @@
     <t>page1-children_seen</t>
   </si>
   <si>
-    <t>nb_children_seen</t>
+    <t>page1-date_Monday</t>
+  </si>
+  <si>
+    <t>date_week</t>
+  </si>
+  <si>
+    <t>page1-monday_seen</t>
+  </si>
+  <si>
+    <t>page1-tuesday_seen</t>
+  </si>
+  <si>
+    <t>page1-wednesday_seen</t>
+  </si>
+  <si>
+    <t>page1-thursday_seen</t>
+  </si>
+  <si>
+    <t>page1-friday_seen</t>
+  </si>
+  <si>
+    <t>u5_attendance_last_week</t>
+  </si>
+  <si>
+    <t>u5_attendance_last_mon</t>
+  </si>
+  <si>
+    <t>u5_attendance_last_tue</t>
+  </si>
+  <si>
+    <t>u5_attendance_last_wed</t>
+  </si>
+  <si>
+    <t>u5_attendance_last_thu</t>
+  </si>
+  <si>
+    <t>u5_attendance_last_fri</t>
+  </si>
+  <si>
+    <t>page1-pox_present</t>
+  </si>
+  <si>
+    <t>page1-probe_present</t>
+  </si>
+  <si>
+    <t>page1-pox_func</t>
+  </si>
+  <si>
+    <t>probe_avail</t>
+  </si>
+  <si>
+    <t>pox_avail</t>
+  </si>
+  <si>
+    <t>pox_functional</t>
   </si>
 </sst>
 </file>
@@ -449,16 +503,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.375" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -504,74 +558,146 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>25</v>
+      <c r="B18" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>